<commit_message>
orangeHRM localhost setUp - xampp setup - orangehrm DB
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sopequipo\Desktop\orangeHRM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EAC2FF-298F-4394-9895-A37422773341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A09E5-EB69-4339-A2F0-63958C4F0857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -34,13 +34,16 @@
     <t>admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>admin1234</t>
+  </si>
+  <si>
+    <t>orangehrm_admin</t>
+  </si>
+  <si>
+    <t>EmployeeAdmin3030**</t>
   </si>
 </sst>
 </file>
@@ -360,26 +363,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -391,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1D553-0E79-4237-8138-32F8F9053BE0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -402,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -410,7 +417,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Database Testing in Selenium
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sopequipo\Desktop\orangeHRM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A09E5-EB69-4339-A2F0-63958C4F0857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B35B43-592E-40AB-BC95-7B665B7309C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="emplVerification" sheetId="3" r:id="rId2"/>
+    <sheet name="invalidLoginData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -44,6 +45,15 @@
   </si>
   <si>
     <t>EmployeeAdmin3030**</t>
+  </si>
+  <si>
+    <t>emp_id</t>
+  </si>
+  <si>
+    <t>emp_name</t>
+  </si>
+  <si>
+    <t>yura</t>
   </si>
 </sst>
 </file>
@@ -363,7 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -395,6 +405,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF774D7A-B67C-4DF3-A8BF-92184AD0BC87}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1D553-0E79-4237-8138-32F8F9053BE0}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>